<commit_message>
Fixed save button, Closing Message Box, and Getting to Comments
</commit_message>
<xml_diff>
--- a/Data/Temp/Yearly-Report-2018-FR065748.xlsx
+++ b/Data/Temp/Yearly-Report-2018-FR065748.xlsx
@@ -16,172 +16,172 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <x:si>
-    <x:t>988142</x:t>
+    <x:t>948453</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>103711</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20742.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>124453</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-01-19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>517728</x:t>
   </x:si>
   <x:si>
     <x:t>Concierge Services</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-01-11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>274058</x:t>
-  </x:si>
-  <x:si>
-    <x:t>54811.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>328870</x:t>
+    <x:t>90055</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18011</x:t>
+  </x:si>
+  <x:si>
+    <x:t>108066</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-03-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>353225</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Professional Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>233059</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46611.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>279671</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-03-19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>731981</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beverages and Catering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>199721</x:t>
+  </x:si>
+  <x:si>
+    <x:t>39944.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>239665</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-03-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>580846</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-04-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77618</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15523.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>93141.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>833079</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-04-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>140362</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28072.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>168434</x:t>
+  </x:si>
+  <x:si>
+    <x:t>681567</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-04-21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>298962</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59792.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>358754</x:t>
   </x:si>
   <x:si>
     <x:t>USD</x:t>
   </x:si>
   <x:si>
-    <x:t>401454</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-01-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>187722</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37544.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>225266</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RON</x:t>
-  </x:si>
-  <x:si>
-    <x:t>736899</x:t>
+    <x:t>875146</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-05-05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47240</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9448</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56688</x:t>
+  </x:si>
+  <x:si>
+    <x:t>313573</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Waste management services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-05-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>119649</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23929.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>143579</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>724233</x:t>
   </x:si>
   <x:si>
     <x:t>Various paper supplies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-01-12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>227842</x:t>
-  </x:si>
-  <x:si>
-    <x:t>45568.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>273410</x:t>
-  </x:si>
-  <x:si>
-    <x:t>568038</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-03-24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>38749</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7749.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>46498.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>580846</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-04-08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>77618</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15523.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>93141.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EUR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>833079</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Beverages and Catering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-04-28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>140362</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28072.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>168434</x:t>
-  </x:si>
-  <x:si>
-    <x:t>681567</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IT Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-04-21</x:t>
-  </x:si>
-  <x:si>
-    <x:t>298962</x:t>
-  </x:si>
-  <x:si>
-    <x:t>59792.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>358754</x:t>
-  </x:si>
-  <x:si>
-    <x:t>875146</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Professional Services</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-05-05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>47240</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9448</x:t>
-  </x:si>
-  <x:si>
-    <x:t>56688</x:t>
-  </x:si>
-  <x:si>
-    <x:t>313573</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Waste management services</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-05-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>119649</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23929.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>143579</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CAD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>724233</x:t>
   </x:si>
   <x:si>
     <x:t>2017-07-11</x:t>
@@ -653,99 +653,99 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
       <x:c r="A3" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
       <x:c r="A4" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="A5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>32</x:v>
@@ -760,7 +760,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
@@ -768,22 +768,22 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="D7" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="E7" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="E7" s="0" t="s">
+      <x:c r="F7" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="F7" s="0" t="s">
+      <x:c r="G7" s="0" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
@@ -791,53 +791,53 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
+      <x:c r="D8" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
+      <x:c r="E8" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="E8" s="0" t="s">
+      <x:c r="F8" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="A9" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s">
+      <x:c r="C9" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
+      <x:c r="D9" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
+      <x:c r="E9" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="E9" s="0" t="s">
+      <x:c r="F9" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="F9" s="0" t="s">
+      <x:c r="G9" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
         <x:v>55</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>56</x:v>
@@ -852,7 +852,7 @@
         <x:v>59</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
@@ -860,7 +860,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>61</x:v>
@@ -875,7 +875,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
@@ -883,7 +883,7 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>66</x:v>
@@ -898,7 +898,7 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
@@ -906,7 +906,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
         <x:v>71</x:v>
@@ -921,7 +921,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
@@ -929,7 +929,7 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>76</x:v>
@@ -944,7 +944,7 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
@@ -952,7 +952,7 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
         <x:v>81</x:v>
@@ -967,7 +967,7 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>